<commit_message>
TestSet1 - some changes needed as all test results diverge or populations die out before the end. Saved record of results
</commit_message>
<xml_diff>
--- a/RewardsV2/HungerRewards.xlsx
+++ b/RewardsV2/HungerRewards.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C10EB4-CB52-454C-86CA-CC1D8ABE16D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB716F69-A826-43B1-A90D-46FE360C22FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,7 +377,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -391,10 +391,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -405,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>

</xml_diff>